<commit_message>
Manual entry of decisions
</commit_message>
<xml_diff>
--- a/src/analysis/python/data/bluebook_missingalternatives.xlsx
+++ b/src/analysis/python/data/bluebook_missingalternatives.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivergiesecke/Dropbox/MPCounterfactual/src/analysis/python/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD76CE33-3551-C84C-9B9B-250BA00B7ACF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F89871-8BA1-6241-975E-57983D20117E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="17560" windowWidth="28020" windowHeight="33440" xr2:uid="{9716385D-8641-8C45-A762-0D006627BD89}"/>
+    <workbookView xWindow="29100" yWindow="7540" windowWidth="28020" windowHeight="28340" xr2:uid="{9716385D-8641-8C45-A762-0D006627BD89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="78">
   <si>
     <t>The Committee could select a 50 basis point reduction in the funds rate at this meeting if it thought an easing of at least this size would prove necessary to promote a return of economic growth to an acceptable pace over time. The resulting 5 percent federal funds rate would imply a real rate of around 3 percent–assuming that inflation expectatio ns are in line with the staff forecast of core PCE p rices. Even if this places the real rate below its long-run equilibrium value, an undershoot may well be needed for a time to counter the effects of the declines in equity wealth, the apparent downward revision to expected near-term returns on capital, a possible
 7
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t xml:space="preserve">If the Committee perceived substantial remaining downside risks to the economic outlook, it instead might select a 25 basis point reduction in the federal funds rate target to 11⁄2 percent. While some recent indicators of capital spending have been encouraging, a sustained revival may be viewed as far from assured. If investors in stock and corporate bond markets came to question the long-term outlook for high-tech industries and the associated trends for economy-wide profit streams and productivity, the resulting downward adjustment in asset prices would set back the recovery of investment and consumption. Moreover, should the news on the labor market remain bad for a while longer, consumer attitudes may turn out to be morefragilethantheyhaveseemedoflate. Whileeasingpolicyanothernotchwould not appreciably reduce the risks of such adverse outcomes, it would at least put the economy on a slightly stronger footing should any of them eventuate. With an intensification of inflation unlikely to pose a threat in the next couple of years, the potential costs of such a policy action might be seen as small when compared with the cumulative shortfall of resource utilization in the staff forecast. Indeed, limiting disinflation at this point might be welcomed for strategic reasons: The risks associated with operating policy at very low nominal interest rates might incline the Committee toward slightly higher inflation than in the Greenbook forecast–as in the “inflation cushion” strategy described above–in order to be able to put in place low real interest rates if need be in the future. Another 1⁄4 percentage point reduction in the federal funds rate, along with a statement that the risks were weighted to the downside, would come as a surprise to market participants, perhaps prompting a sense that the economic outlook was a little weaker than previously perceived. As a result, some immediate reduction in long-term as well as short-term interest rates likely would occur. </t>
-  </si>
-  <si>
-    <t>If the Committee reads the strength of recent economic indicators as signaling that lasting economic growth above potential is a distinct likelihood, it might wish to hold the funds rate unchanged and move the balance of risks toward heightened inflation pressures. With the economy seeming to have regained its footing, the Committee might view a balance toward inflation as especially appropriate in light of the un sustainably low level of the real fund s rate, the recent up tick in measures of inflation expectations based on Treasury inflation-indexed securities, and the possibility that sharp increases in oil prices could feed through to prices and wages more generally. Indeed, the surprising resilience exhibited by the economy of late raises the possibility that spending may snap back more rapidly than in the Greenbook. If the Committee were especially concerned that, if it did not move promptly to begin to restore the funds rate to more sustainable levels, inflation pressures could build over time to the point that they would be difficult to contain, it might even choose to implement a quarter-point increase in the target funds rate along with a balance of risks weighted toward inflation pressures. In particular, the apparent turnaround of demand in the high-tech sector, favorable news on productivity, accelerator effects stemming from the recent pickup in output growth, and the business tax incentives included in the fiscal stimulus package might be imparting an even more sizable impetus to investment spending than in the staff forecast. Forces such as these help to explain why some measures of the equilibrium real funds rate have been boosted as much as a half a percentage point over the intermeeting period (Chart 4). Such an increase in estimates of the equilibrium real funds rate im plies that just ma intaining the sam e degree of po licy stimulus w ould require increasing the nominal funds rate target. Market participants do not expect a move to a balance of risks toward inflation pressures at this meeting, much less one accompanied by a quarter-point increase in the target funds rate. As a result, either choice would push interest rates higher across the term structure while equities could come under heavy selling pressure. The extent of the market reaction could be sizable and, of course , would depend importantly on the wording of the annou ncement and the associated m arket perceptionsaboutthefuturecourseofpolicy. In particular, the reaction in markets could be attenuated if the wording of the announcement emphasized that the Committee viewed itself as merely unwinding some of the insurance it had taken out late last year at a time of unusual uncertainty, and that it intended to wait thereafter, rather than embark on a path that would promptly realign the real interest rate to a more normal level.</t>
   </si>
   <si>
     <t>alt4</t>
@@ -340,6 +337,12 @@
   </si>
   <si>
     <t>change</t>
+  </si>
+  <si>
+    <t>If the Committee reads the strength of recent economic indicators as signaling that lasting economic growth above potential is a distinct likelihood, it might wish to hold the funds rate unchanged and move the balance of risks toward heightened inflation pressures. With the economy seeming to have regained its footing, the Committee might view a balance toward inflation as especially appropriate in light of the un sustainably low level of the real fund s rate, the recent up tick in measures of inflation expectations based on Treasury inflation-indexed securities, and the possibility that sharp increases in oil prices could feed through to prices and wages more generally. Indeed, the surprising resilience exhibited by the economy of late raises the possibility that spending may snap back more rapidly than in the Greenbook. If the Committee were especially concerned that, if it did not move promptly to begin to restore the funds rate to more sustainable levels, inflation pressures could build over time to the point that they would be difficult to contain, it might even choose to implement a quarter-point increase in the target funds rate along with a balance of risks weighted toward inflation pressures. In particular, the apparent turnaround of demand in the high-tech sector, favorable news on productivity, accelerator effects stemming from the recent pickup in output growth, and the business tax incentives included in the fiscal stimulus package might be imparting an even more sizable impetus to investment spending than in the staff forecast. Forces such as these help to explain why some measures of the equilibrium real funds rate have been boosted as much as a half a percentage point over the intermeeting period (Chart 4). Such an increase in estimates of the equilibrium real funds rate im plies that just ma intaining the same degree of policy stimulus would require increasing the nominal funds rate target. Market participants do not expect a move to a balance of risks toward inflation pressures at this meeting, much less one accompanied by a quarter-point increase in the target funds rate. As a result, either choice would push interest rates higher across the term structure while equities could come under heavy selling pressure. The extent of the market reaction could be sizable and, of course , would depend importantly on the wording of the announcement and the associated market perceptions about the future course of policy. In particular, the reaction in markets could be attenuated if the wording of the announcement emphasized that the Committee viewed itself as merely unwinding some of the insurance it had taken out late last year at a time of unusual uncertainty, and that it intended to wait thereafter, rather than embark on a path that would promptly realign the real interest rate to a more normal level.</t>
+  </si>
+  <si>
+    <t>If as in the Greenbook ,  the Committee sees inflation pressures as likely to remain muted and expects output to grow only somewhat faster than potential supply, then it might well choose to indicate that risks to the outlook are balanced over the “foreseeable future.” In an environment of heightened uncertainty, in particular, the Committee may view the horizon at which the foreseeable future ends to be shorter than the date at which the Greenbook assumes tightening begins. Even if the Committee is fairly certain its next action will be to tighten, such a statement could still be appropriate if the odds on some disappointment on economic performance in the near term roughly balance the possibility that inflation may ultimately pick up. An unchanged target federal funds rate, along with a statement indicating that the risks to the outlook are balanced, would match investors’ expectations, and so would likely have little effect on financial markets.</t>
   </si>
 </sst>
 </file>
@@ -751,32 +754,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C35FE6-3980-E94D-9EE2-3C2A0EB4F129}">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="3" max="3" width="62.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>73</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>74</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>75</v>
-      </c>
-      <c r="E1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="409.6">
@@ -790,7 +794,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2">
         <v>-0.5</v>
@@ -804,10 +808,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3">
         <v>-0.75</v>
@@ -821,10 +825,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4">
         <v>-0.25</v>
@@ -838,10 +842,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5">
         <v>-0.5</v>
@@ -858,7 +862,7 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6">
         <v>-0.25</v>
@@ -875,7 +879,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7">
         <v>-0.75</v>
@@ -889,10 +893,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -909,7 +913,7 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9">
         <v>-0.25</v>
@@ -926,7 +930,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10">
         <v>-0.5</v>
@@ -940,10 +944,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -960,7 +964,7 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E12">
         <v>-0.25</v>
@@ -977,7 +981,7 @@
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13">
         <v>-0.5</v>
@@ -994,7 +998,7 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14">
         <v>-0.5</v>
@@ -1008,10 +1012,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15">
         <v>-0.25</v>
@@ -1028,7 +1032,7 @@
         <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1045,7 +1049,7 @@
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E17">
         <v>-0.25</v>
@@ -1062,7 +1066,7 @@
         <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E18">
         <v>-0.5</v>
@@ -1079,7 +1083,7 @@
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1096,7 +1100,7 @@
         <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20">
         <v>-0.25</v>
@@ -1110,10 +1114,10 @@
         <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E21">
         <v>-0.5</v>
@@ -1130,7 +1134,7 @@
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1147,7 +1151,7 @@
         <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E23">
         <v>-0.25</v>
@@ -1161,10 +1165,10 @@
         <v>1</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1178,10 +1182,10 @@
         <v>2</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E25">
         <v>-0.25</v>
@@ -1195,10 +1199,10 @@
         <v>4</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1209,13 +1213,13 @@
         <v>37334</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="D27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1229,10 +1233,10 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1246,47 +1250,47 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="409.6">
+    <row r="30" spans="1:5">
       <c r="A30" s="2">
         <v>37383</v>
       </c>
       <c r="B30" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="409.6">
+      <c r="A31" s="2">
+        <v>37383</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30">
+      <c r="C31" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31">
         <v>0.25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="2">
-        <v>37432</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D31" t="s">
-        <v>54</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1294,50 +1298,50 @@
         <v>37432</v>
       </c>
       <c r="B32" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E32">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="2">
         <v>37432</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33">
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="2">
+        <v>37432</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C33" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33" t="s">
-        <v>56</v>
-      </c>
-      <c r="E33">
+      <c r="C34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34">
         <v>0.25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="409.6">
-      <c r="A34" s="2">
-        <v>37481</v>
-      </c>
-      <c r="B34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" t="s">
-        <v>54</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="409.6">
@@ -1345,13 +1349,13 @@
         <v>37481</v>
       </c>
       <c r="B35" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="D35" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -1361,34 +1365,34 @@
       <c r="A36" s="2">
         <v>37481</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="409.6">
+      <c r="A37" s="2">
+        <v>37481</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D36" t="s">
-        <v>56</v>
-      </c>
-      <c r="E36">
-        <v>-0.25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="409.6">
-      <c r="A37" s="6">
-        <v>37523</v>
-      </c>
-      <c r="B37" t="s">
-        <v>1</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D37" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="409.6">
@@ -1396,13 +1400,13 @@
         <v>37523</v>
       </c>
       <c r="B38" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="D38" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -1412,34 +1416,34 @@
       <c r="A39" s="6">
         <v>37523</v>
       </c>
-      <c r="B39" s="8" t="s">
-        <v>4</v>
+      <c r="B39" t="s">
+        <v>2</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D39" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E39">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="409.6">
       <c r="A40" s="6">
-        <v>37566</v>
-      </c>
-      <c r="B40" t="s">
-        <v>1</v>
+        <v>37523</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="D40" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="409.6">
@@ -1447,50 +1451,50 @@
         <v>37566</v>
       </c>
       <c r="B41" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="D41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E41">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="409.6">
       <c r="A42" s="6">
         <v>37566</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" t="s">
+        <v>54</v>
+      </c>
+      <c r="E42">
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="409.6">
+      <c r="A43" s="6">
+        <v>37566</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D42" t="s">
-        <v>56</v>
-      </c>
-      <c r="E42">
+      <c r="C43" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" t="s">
+        <v>55</v>
+      </c>
+      <c r="E43">
         <v>-0.5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="409.6">
-      <c r="A43" s="2">
-        <v>37600</v>
-      </c>
-      <c r="B43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D43" t="s">
-        <v>54</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="409.6">
@@ -1498,33 +1502,33 @@
         <v>37600</v>
       </c>
       <c r="B44" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D44" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E44">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="409.6">
       <c r="A45" s="2">
-        <v>37649</v>
+        <v>37600</v>
       </c>
       <c r="B45" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D45" t="s">
         <v>54</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="409.6">
@@ -1532,84 +1536,84 @@
         <v>37649</v>
       </c>
       <c r="B46" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D46" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E46">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="409.6">
       <c r="A47" s="2">
-        <v>37698</v>
+        <v>37649</v>
       </c>
       <c r="B47" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D47" t="s">
         <v>54</v>
       </c>
       <c r="E47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="17">
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="409.6">
       <c r="A48" s="2">
         <v>37698</v>
       </c>
       <c r="B48" t="s">
-        <v>2</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>36</v>
+        <v>1</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D48" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E48">
-        <v>-0.25</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="409.6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="17">
       <c r="A49" s="2">
         <v>37698</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D49" t="s">
+        <v>54</v>
+      </c>
+      <c r="E49">
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="409.6">
+      <c r="A50" s="2">
+        <v>37698</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D49" t="s">
-        <v>56</v>
-      </c>
-      <c r="E49">
+      <c r="C50" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D50" t="s">
+        <v>55</v>
+      </c>
+      <c r="E50">
         <v>-0.5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="409.6">
-      <c r="A50" s="6">
-        <v>37747</v>
-      </c>
-      <c r="B50" t="s">
-        <v>1</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D50" t="s">
-        <v>54</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="409.6">
@@ -1617,27 +1621,27 @@
         <v>37747</v>
       </c>
       <c r="B51" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D51" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E51">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="409.6">
       <c r="A52" s="6">
-        <v>37796</v>
+        <v>37747</v>
       </c>
       <c r="B52" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D52" t="s">
         <v>54</v>
@@ -1651,47 +1655,47 @@
         <v>37796</v>
       </c>
       <c r="B53" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D53" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E53">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="409.6">
       <c r="A54" s="6">
         <v>37796</v>
       </c>
-      <c r="B54" s="8" t="s">
-        <v>4</v>
+      <c r="B54" t="s">
+        <v>2</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D54" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E54">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="409.6">
       <c r="A55" s="6">
-        <v>37845</v>
-      </c>
-      <c r="B55" t="s">
-        <v>1</v>
+        <v>37796</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D55" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -1702,33 +1706,33 @@
         <v>37845</v>
       </c>
       <c r="B56" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D56" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E56">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="409.6">
       <c r="A57" s="6">
-        <v>37880</v>
+        <v>37845</v>
       </c>
       <c r="B57" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="D57" t="s">
         <v>54</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="409.6">
@@ -1736,33 +1740,33 @@
         <v>37880</v>
       </c>
       <c r="B58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="D58" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E58">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="409.6">
       <c r="A59" s="6">
-        <v>37922</v>
+        <v>37880</v>
       </c>
       <c r="B59" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D59" t="s">
         <v>54</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="409.6">
@@ -1770,33 +1774,33 @@
         <v>37922</v>
       </c>
       <c r="B60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D60" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E60">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="409.6">
       <c r="A61" s="6">
-        <v>37964</v>
+        <v>37922</v>
       </c>
       <c r="B61" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D61" t="s">
         <v>54</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="409.6">
@@ -1804,33 +1808,33 @@
         <v>37964</v>
       </c>
       <c r="B62" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D62" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E62">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="409.6">
       <c r="A63" s="6">
-        <v>38013</v>
+        <v>37964</v>
       </c>
       <c r="B63" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D63" t="s">
         <v>54</v>
       </c>
       <c r="E63">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="409.6">
@@ -1838,32 +1842,49 @@
         <v>38013</v>
       </c>
       <c r="B64" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D64" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E64">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="409.6">
       <c r="A65" s="6">
         <v>38013</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B65" t="s">
+        <v>2</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D65" t="s">
+        <v>54</v>
+      </c>
+      <c r="E65">
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="409.6">
+      <c r="A66" s="6">
+        <v>38013</v>
+      </c>
+      <c r="B66" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D65" t="s">
-        <v>56</v>
-      </c>
-      <c r="E65">
+      <c r="C66" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D66" t="s">
+        <v>55</v>
+      </c>
+      <c r="E66">
         <v>0.25</v>
       </c>
     </row>

</xml_diff>